<commit_message>
Updated Event Analysis scripts and SAS programs
</commit_message>
<xml_diff>
--- a/newman_events_2017/documentation/mm10_event_analysis_rsem_quantification.xlsx
+++ b/newman_events_2017/documentation/mm10_event_analysis_rsem_quantification.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yamanto\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RSEM" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="RSEM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
   <si>
     <t>Event analysis – RSEM quantification</t>
   </si>
@@ -76,7 +80,7 @@
     <t>done</t>
   </si>
   <si>
-    <t>Export list of transcripts for RSEM </t>
+    <t>Export list of transcripts for RSEM</t>
   </si>
   <si>
     <t>SAS</t>
@@ -88,8 +92,7 @@
 2. All Pacbio (again, raw input)
 3. all 73K transcripts detected
 4. exp transcripts with all features detected at APN&gt;0
-5. exp transcripts with at least 75% features detected at APN&gt;0
-</t>
+5. exp transcripts with at least 75% features detected at APN&gt;0</t>
   </si>
   <si>
     <t>analysis_subset_transcripts_for_rsem.sas</t>
@@ -112,8 +115,7 @@
 references/refseq_mm10_exp_transcripts_100perc_dtct_gene2xs.txt"
 /references/refseq_mm10_exp_transcripts_75perc_dtct_apn5_gene2xs.txt"
 references/refseq_mm10_exp_transcripts_75perc_dtct_apn10_gene2xs.txt
-references/pacbio_mm10_gene2xs.txt"
-</t>
+references/pacbio_mm10_gene2xs.txt"</t>
   </si>
   <si>
     <t>Subset FASTA for selected sets of transcripts</t>
@@ -144,8 +146,7 @@
 references/refseq_mm10_exp_transcripts_75perc_dtct.fa
 references/refseq_mm10_exp_transcripts_100perc_dtct.fa
 references/refseq_mm10_exp_transcripts_75perc_dtct_apn5.fa
-references/refseq_mm10_exp_transcripts_75perc_dtct_apn10.fa
-</t>
+references/refseq_mm10_exp_transcripts_75perc_dtct_apn10.fa</t>
   </si>
   <si>
     <t>Build references</t>
@@ -163,8 +164,7 @@
 rsem-prepare-reference --bowtie -p 2 \
                        --transcript-to-gene-map $REF/${GENE2XS} \
                        $REF/${FASTA} \
-                       $REF/${RSEMREF}
-</t>
+                       $REF/${RSEMREF}</t>
   </si>
   <si>
     <t>run_rsem_build_references.sbatch</t>
@@ -180,8 +180,7 @@
 refseq_mm10_exp_transcripts_100perc_dtct
 pacbio_mm10
 refseq_mm10_exp_transcripts_75perc_dtct_apn5
-refseq_mm10_exp_transcripts_75perc_dtct_apn10
-</t>
+refseq_mm10_exp_transcripts_75perc_dtct_apn10</t>
   </si>
   <si>
     <t>${REFSET}_RSEM
@@ -192,8 +191,7 @@
 refseq_mm10_exp_transcripts_100perc_dtct
 pacbio_mm10
 refseq_mm10_exp_transcripts_75perc_dtct_apn5
-refseq_mm10_exp_transcripts_75perc_dtct_apn10
-</t>
+refseq_mm10_exp_transcripts_75perc_dtct_apn10</t>
   </si>
   <si>
     <t>Run RSEM</t>
@@ -211,8 +209,7 @@
                           --estimate-rspd \
                           --fragment-length-mean 80 \
                           --fragment-length-sd 50 \
-                          ${READS} ${REF}/${RSEMREF} ${OUTPUT}
-</t>
+                          ${READS} ${REF}/${RSEMREF} ${OUTPUT}</t>
   </si>
   <si>
     <t>run_rsem_calc_expression.sbatch</t>
@@ -258,8 +255,7 @@
 refseq_mm10_exp_transcripts_100perc_dtct
 refseq_mm10_exp_transcripts_75perc_dtct
 refseq_mm10_exp_transcripts_75perc_dtct_apn5
-refseq_mm10_exp_transcripts_75perc_dtct_apn10
-</t>
+refseq_mm10_exp_transcripts_75perc_dtct_apn10</t>
   </si>
   <si>
     <t>event.rsem_&amp;outname.
@@ -270,11 +266,10 @@
 events_exp_100perc
 events_exp_75perc
 events_exp_75perc_apn5
-events_exp_75perc_apn10
-</t>
-  </si>
-  <si>
-    <t>                                        Non-log         Log
+events_exp_75perc_apn10</t>
+  </si>
+  <si>
+    <t>Non-log         Log
 LIST            STAT            N       R2      SpRho   R2      SpRho
 Refseq all      TPM             128631  0.96893 0.78823 0.97390 0.78823
 PacBio all      TPM             16104   0.94138 0.95392 0.95928 0.95392
@@ -282,45 +277,20 @@
 EA 100%         TPM             14734   0.96559 0.95207 0.97238 0.95207
 EA 75%          TPM             34622   0.96645 0.88494 0.97012 0.88494
 EA 75%, APN5    TPM             13740   0.96557 0.95237 0.97192 0.95237
-EA 75%, APN10   TPM             9879    0.96900 0.96291 0.97376 0.96291
-</t>
+EA 75%, APN10   TPM             9879    0.96900 0.96291 0.97376 0.96291</t>
   </si>
   <si>
     <t>Bin transcripts by RSEM TPM and re-calc concordance</t>
   </si>
   <si>
     <t>Export RSEM FPKM data for making plots -- I also want to bin transcripts into the same 3 bins as
-  in the SQANTI paper: min-Q1, Q1-Q3, Q3-max </t>
+  in the SQANTI paper: min-Q1, Q1-Q3, Q3-max</t>
   </si>
   <si>
     <t>analysis_rsem_export_counts_for_plots.sas</t>
   </si>
   <si>
-    <t>event.rsem_&amp;datain
-&amp;datain=
-refseq_all
-pacbio_all
-events_exp_any
-events_exp_100perc
-events_exp_75perc
-events_exp_75perc_apn5
-events_exp_75perc_apn10
-</t>
-  </si>
-  <si>
-    <t>analysis_output/rsem_fpkm_&amp;datain..csv
-&amp;datain=
-refseq_all
-pacbio_all
-events_exp_any
-events_exp_100perc
-events_exp_75perc
-events_exp_75perc_apn5
-events_exp_75perc_apn10
-</t>
-  </si>
-  <si>
-    <t>                Bin1                            Bin2                            Bin3
+    <t>Bin1                            Bin2                            Bin3
                 N       r2      r2(log) rho     N       r2      r2(log) rho     N       r2      r2(log) rho
 RefSeq All      80455   0.11126 0.11427 0.28539 31757   0.49074 0.53274 0.40681 16419   0.96805 0.94075 0.89585 
 Event Exp       39553   0.07968 0.08290 0.25646 22618   0.52411 0.57104 0.44153 11364   0.96581 0.94602 0.90768
@@ -328,41 +298,27 @@
 Event 75% APN5  4841    0.38807 0.48099 0.58100 5931    0.79641 0.76827 0.82718 2968    0.96243 0.95035 0.92521
 Event 100%      4414    0.39839 0.48106 0.57050 6880    0.79014 0.78045 0.82303 3440    0.96296 0.94892 0.92393
 Event 75% APN10 3335    0.44808 0.56321 0.63960 4363    0.83023 0.79988 0.86259 2181    0.96557 0.94797 0.92108
-PacBio All      4779    0.53537 0.66089 0.68146 7550    0.73962 0.68778 0.78093 3775    0.93748 0.92512 0.88866
-</t>
+PacBio All      4779    0.53537 0.66089 0.68146 7550    0.73962 0.68778 0.78093 3775    0.93748 0.92512 0.88866</t>
   </si>
   <si>
     <t>Data for BA plots</t>
   </si>
   <si>
-    <t> BA plots for each RSEM output. I am going to calculate the data needed for plots here then export
+    <t>BA plots for each RSEM output. I am going to calculate the data needed for plots here then export
    to python for plotting
-   Put in macro so I can iterate through the data
-</t>
+   Put in macro so I can iterate through the data</t>
   </si>
   <si>
     <t>analysis_rsem_calc_data_for_ba_plots.sas</t>
   </si>
   <si>
-    <t>analysis_output/rsem_ba_plot_data_&amp;datain..csv
-&amp;datain=
-refseq_all
-pacbio_all
-events_exp_any
-events_exp_100perc
-events_exp_75perc
-events_exp_75perc_apn5
-events_exp_75perc_apn10
-</t>
-  </si>
-  <si>
     <t>Export caounts for plots (v2)</t>
   </si>
   <si>
     <t>analysis_rsem_export_counts_for_plots_jrbn2.sas</t>
   </si>
   <si>
-    <t>                Bin1                            Bin2                            Bin3
+    <t>Bin1                            Bin2                            Bin3
                 N       r2      r2(log) rho     N       r2      r2(log) rho     N       r2      r2(log) rho
 RefSeq All      80455   0.11126 0.11427 0.28539 31757   0.49074 0.53274 0.40681 16419   0.96805 0.94075 0.89585 
 Event Exp       39553   0.07968 0.08290 0.25646 22618   0.52411 0.57104 0.44153 11364   0.96581 0.94602 0.90768
@@ -370,40 +326,250 @@
 9Event 75% APN5 4841    0.38807 0.48099 0.58100 5931    0.79641 0.76827 0.82718 2968    0.96243 0.95035 0.92521
 Event 100%      4414    0.39839 0.48106 0.57050 6880    0.79014 0.78045 0.82303 3440    0.96296 0.94892 0.92393
 Event 75% APN10 3335    0.44808 0.56321 0.63960 4363    0.83023 0.79988 0.86259 2181    0.96557 0.94797 0.92108
-PacBio All      4779    0.53537 0.66089 0.68146 7550    0.73962 0.68778 0.78093 3775    0.93748 0.92512 0.88866
+PacBio All      4779    0.53537 0.66089 0.68146 7550    0.73962 0.68778 0.78093 3775    0.93748 0.92512 0.88866</t>
+  </si>
+  <si>
+    <t>analysis_mouse_calc_rep_concordance_absoluate_threshold_02jrbn.sas</t>
+  </si>
+  <si>
+    <t>analysis_mouse_calc_rep_ccv_by_tpm_bin.sas</t>
+  </si>
+  <si>
+    <t>analysis_import_rsem_estimates_mm10_calc_CV_by_tpm_bin_and_sample.sas</t>
+  </si>
+  <si>
+    <t>analysis_mouse_calc_rep_agreement_kappa_0_vs_any.sas</t>
+  </si>
+  <si>
+    <t>Bin transcripts by log-TPM and calculate correlation</t>
+  </si>
+  <si>
+    <t>Export RSEM TPM data for making plots -- I also want to bin transcripts into the same 3 bins as
+  in the SQANTI paper: min-Q1, Q1-Q3, Q3-max</t>
+  </si>
+  <si>
+    <t>event.rsem_&amp;datain
+&amp;datain=
+refseq_all
+pacbio_all
+pacbio_apn0
+pacbio_apn5
+pacbio_apn10
+events_exp_any
+events_exp_100perc
+events_exp_100perc_apn5
+events_exp_100perc_apn10
+events_exp_75perc
+events_exp_75perc_apn5
+events_exp_75perc_apn10
+events_exp_50perc
+events_exp_50perc_apn5
+events_exp_50perc_apn10</t>
+  </si>
+  <si>
+    <t>analysis_output/rsem_tpm_&amp;datain..csv
+&amp;datain=
+refseq_all
+pacbio_all
+pacbio_apn0
+pacbio_apn5
+pacbio_apn10
+events_exp_any
+events_exp_100perc
+events_exp_100perc_apn5
+events_exp_100perc_apn10
+events_exp_75perc
+events_exp_75perc_apn5
+events_exp_75perc_apn10
+events_exp_50perc
+events_exp_50perc_apn5
+events_exp_50perc_apn10</t>
+  </si>
+  <si>
+    <t>analysis_output/rsem_fpkm_&amp;datain..csv
+&amp;datain=
+refseq_all
+pacbio_all
+pacbio_apn0
+pacbio_apn5
+pacbio_apn10
+events_exp_any
+events_exp_100perc
+events_exp_100perc_apn5
+events_exp_100perc_apn10
+events_exp_75perc
+events_exp_75perc_apn5
+events_exp_75perc_apn10
+events_exp_50perc
+events_exp_50perc_apn5
+events_exp_50perc_apn10</t>
+  </si>
+  <si>
+    <t>analysis_output/rsem_ba_plot_data_&amp;datain..csv
+&amp;datain=
+refseq_all
+pacbio_all
+pacbio_apn0
+pacbio_apn5
+pacbio_apn10
+events_exp_any
+events_exp_100perc
+events_exp_100perc_apn5
+events_exp_100perc_apn10
+events_exp_75perc
+events_exp_75perc_apn5
+events_exp_75perc_apn10
+events_exp_50perc
+events_exp_50perc_apn5
+events_exp_50perc_apn10</t>
+  </si>
+  <si>
+    <t>tpm_bin</t>
+  </si>
+  <si>
+    <t>Export RSEM TPM data for making plots. I am binning transcripts into bin:
+bin 0 : mean log TPM = 0
+bin 1 : minimum log TPM across reps is &lt; 0.5
+bin 2 : minimum log TPM across reps is between 0.5 and 2
+bin 3 : minimum log TPM across reps is between 2 and 4
+bin 4 : minimum log TPM across reps is 4 or greater
+Then for each I am calculating the r2 between reps
+ for each bin</t>
+  </si>
+  <si>
+    <t>Bin transcripts by log-TPM and calculate CV</t>
+  </si>
+  <si>
+    <t>analysis_output/rsem_tpm_&amp;datain..csv
+&amp;datain=
+refseq_all
+pacbio_all
+pacbio_apn0
+pacbio_apn5
+pacbio_apn10
+events_exp_any
+events_exp_100perc
+events_exp_100perc_apn5
+events_exp_100perc_apn10
+events_exp_75perc
+events_exp_75perc_apn5
+events_exp_75perc_apn10
+events_exp_50perc
+events_exp_50perc_apn5
+events_exp_50perc_apn10
+analysis_output/CV_by_TPM_bin_by_transcript_set.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     PACBIO          REFSEQ_ALL              EA_100_APN0     EA_75_APN5
+BIN     N       CV_MEAN N       CV_MEAN N       CV_MEAN N       CV_MEAN
+0       1002    n/a     62940   n/a     970     n/a     1868    n/a
+1       1635    76.3796 45378   128.767 3377    87.1348 2715    81.0323
+2       4307    29.3791 12226   36.347  4426    33.0444 3295    33.1822
+3       6649    18.4165 5940    19.045  4032    18.5452 3925    18.2734
+4       2511    17.7129 2147    18.859  1929    19.7183 1937    19.8243
+Bins:
+0 = average TPM is 0 (no expression)
+1 = minimum TPM is &lt;0.5 (very low expression)
+2 = minimum TPM is &lt;2   (low expression)
+3 = minimum TPM is &lt;4   (moderate expression)
+4 = minimum TPM is ge 4 (high expression)
 </t>
+  </si>
+  <si>
+    <t>Re-import RSEM estimates, bin transcripts by log-TPM and calculate within-bin/within-sample CV</t>
+  </si>
+  <si>
+    <t>Export RSEM TPM data for making plots. I am binning transcripts into bin:
+bin 0 : mean log TPM = 0
+bin 1 : minimum log TPM across reps is &lt; 0.5
+bin 2 : minimum log TPM across reps is between 0.5 and 2
+bin 3 : minimum log TPM across reps is between 2 and 4
+bin 4 : minimum log TPM across reps is 4 or greater
+Then for each I am calculating the CV of the mean log-TPM between reps for each bin (NPCs only)</t>
+  </si>
+  <si>
+    <t>analysis_output/rsem_output/&amp;datain._NSC1.isoforms.results
+analysis_output/rsem_output/&amp;datain._NSC2.isoforms.results
+analysis_output/rsem_output/&amp;datain._OLD1.isoforms.results
+analysis_output/rsem_output/&amp;datain._OLD2.isoforms.results
+&amp;datain=
+refseq_all
+pacbio_all
+pacbio_apn0
+pacbio_apn5
+pacbio_apn10
+events_exp_any
+events_exp_100perc
+events_exp_100perc_apn5
+events_exp_100perc_apn10
+events_exp_75perc
+events_exp_75perc_apn5
+events_exp_75perc_apn10
+events_exp_50perc
+events_exp_50perc_apn5
+events_exp_50perc_apn10</t>
+  </si>
+  <si>
+    <t>Export RSEM TPM data for making plots. I am binning transcripts into bin:
+bin 0 : log TPM = 0
+bin 1 : log TPM within a rep is &lt; 0.5
+bin 2 : log TPM within a rep is between 0.5 and 2
+bin 3 : log TPM within a rep is between 2 and 4
+bin 4 : log TPM within a rep is 4 or greater
+Then for each I am calculating the CV within reps for each bin</t>
+  </si>
+  <si>
+    <t>Calculate simple agreement between NPC reps per log-TPM bin</t>
+  </si>
+  <si>
+    <t>analysis_output/agreement_stats_by_transcript_set.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analysis_output/CV_and_counts_by_tpm_bin_and_sample_alldata.csv 
+</t>
+  </si>
+  <si>
+    <t>Calculate the simple agreement as a proportion of transcripts detected in only one rep vs the total number of transcripts (NPC only)
+%disagreement = ( NPC rep 1 only + NPC rep 2 only)/(all transcripts in transcript set)
+Bins:
+bin 0 : log TPM = 0
+bin 1 : log TPM within a rep is &lt; 0.5
+bin 2 : log TPM within a rep is between 0.5 and 2
+bin 3 : log TPM within a rep is between 2 and 4
+bin 4 : log TPM within a rep is 4 or greater</t>
+  </si>
+  <si>
+    <t>Make concordance/BA plots plots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make correlation and Blant Altman plots for illustrating rep-to-rep concordance between NPC samples, coloring transcripts by log_TPM bin
+bin 0 : mean log TPM = 0 (black)
+bin 1 : minimum log TPM across reps is &lt; 0.5 (red)
+bin 2 : minimum log TPM across reps is between 0.5 and 2 (orange)
+bin 3 : minimum log TPM across reps is between 2 and 4 (yellow)
+bin 4 : minimum log TPM across reps is 4 or greater (blue)
+Note: while both plots are made, only the BA plots are useful and used
+</t>
+  </si>
+  <si>
+    <t>plot_concordance_plots_for_tpm_estimates.py</t>
+  </si>
+  <si>
+    <t>make_concordance_plots_for_tpm_estimates.sh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -417,8 +583,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -434,7 +600,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -442,107 +608,365 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:L14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.1836734693878"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.5714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.5510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.2908163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="55.3214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="11.5703125"/>
+    <col min="2" max="2" width="70.42578125"/>
+    <col min="3" max="3" width="11.5703125"/>
+    <col min="4" max="4" width="61.7109375"/>
+    <col min="5" max="5" width="45.5703125"/>
+    <col min="6" max="6" width="38.140625"/>
+    <col min="7" max="7" width="31.5703125"/>
+    <col min="8" max="8" width="32.5703125"/>
+    <col min="9" max="9" width="21.28515625"/>
+    <col min="10" max="10" width="55.28515625"/>
+    <col min="11" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="43.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +981,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4"/>
@@ -568,7 +992,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="28.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
@@ -583,7 +1007,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="28.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
@@ -598,7 +1022,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="70.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>6</v>
@@ -613,7 +1037,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -644,20 +1068,20 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:12" ht="369.75" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="8" t="s">
@@ -667,14 +1091,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="84.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -683,7 +1107,7 @@
       <c r="E8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="8" t="s">
@@ -693,14 +1117,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:12" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -709,7 +1133,7 @@
       <c r="E9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>35</v>
       </c>
       <c r="G9" s="8" t="s">
@@ -719,14 +1143,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="227.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:12" ht="318.75" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -735,30 +1159,30 @@
       <c r="E10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" t="s">
         <v>41</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:12" ht="229.5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
         <v>46</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -771,86 +1195,209 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="132.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:12" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" t="s">
         <v>52</v>
       </c>
       <c r="G12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="8" t="s">
+    </row>
+    <row r="13" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
         <v>54</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="144.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="B14" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="132.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="306" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J14" s="8" t="s">
+      <c r="G17" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="331.5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" t="s">
         <v>62</v>
       </c>
+      <c r="G18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="331.5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="280.5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>